<commit_message>
added saving.html & saving.xlsx
</commit_message>
<xml_diff>
--- a/Excel/saving.xlsx
+++ b/Excel/saving.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Websites\audacity-mr\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -97,86 +102,86 @@
     <t>|&lt; Back to: Getting Started</t>
   </si>
   <si>
-    <t>जतन करीत आहे - ऑडसिटी मॅन्युअल</t>
-  </si>
-  <si>
-    <t>बचत</t>
-  </si>
-  <si>
-    <t>ऑडसिटी डेव्हलपमेंट मॅन्युअल वरुन</t>
-  </si>
-  <si>
-    <t>येथे जा: सुचालन, शोध</t>
-  </si>
-  <si>
-    <t>आपण सोडल्याप्रमाणे सर्व ट्रॅक आणि संपादनांसह ऑडॅसिटीमधील आपल्या अपूर्ण कामात परत येण्यासाठी, ऑडसीटी प्रकल्प जतन करा.</t>
-  </si>
-  <si>
-    <t>आपले सध्याचे कार्य अन्य मीडिया अनुप्रयोगांमध्ये प्ले करण्यासाठी किंवा इतरांना आपले कार्य पाठविण्याकरिता, आपल्याला डब्ल्यूएव्ही किंवा एमपी 3 सारख्या ऑडिओ फाईलची निर्यात करण्याची आवश्यकता आहे.</t>
-  </si>
-  <si>
-    <t>आपल्याला एखादी फाइल जतन करण्यात समस्या येत असल्यास, प्रकल्प वाचवण्याविषयी नेहमी विचारले जाणारे प्रश्न पहा जे काही वारंवार विचारल्या जाणा .्या प्रश्नांची उत्तरे देतात.</t>
-  </si>
-  <si>
     <t>जतन करा</t>
   </si>
   <si>
     <t>प्रकल्प वाचविण्यासाठी तीन मुख्य आज्ञा आहेतः</t>
   </si>
   <si>
-    <t>फाइल&gt; प्रकल्प जतन करा&gt; सेव्ह प्रोजेक्टमध्ये एक .aup प्रोजेक्ट फाईल आणि वास्तविक ऑडिओ असलेली _डेटा फोल्डर जतन होते.</t>
-  </si>
-  <si>
-    <t>फाईल&gt; प्रकल्प जतन करा&gt; प्रोजेक्टची लॉसलेस कॉपी जतन करा ... आपल्या विद्यमान प्रोजेक्टला नवीन नावाने सेव्ह करू देते, आपला विद्यमान प्रकल्प सतत संपादनासाठी खुला ठेवून.</t>
-  </si>
-  <si>
-    <t>फाइल&gt; प्रकल्प जतन करा&gt; प्रकल्प म्हणून जतन करा ... आपल्याला विद्यमान प्रकल्प एका नवीन नावाने जतन करू देते, नवीन प्रकल्प उघडेल आणि जुना प्रकल्प बंद करा.</t>
-  </si>
-  <si>
-    <t>हे .aup फाइल आणि _डेटा फोल्डर जतन करते किंवा अद्यतनित करते. प्रोजेक्ट सेव्ह करणे आपल्याला सर्व संपादने आणि रेकॉर्ड केलेले / आयातित ट्रॅकसह, अपूर्ण काम वाचवू देते आणि नंतर ऑडसेटमध्ये जसे होते तसे होते तसेच (पूर्ववत इतिहास वगळता) पुन्हा उघडू देते. कोणत्याही प्रकारची फाईल सेव्हिंग प्रमाणे, काही अक्षरे .aup फाईलच्या नावावर वापरता येणार नाहीत जर त्या ऑपरेटिंग सिस्टमसाठी आरक्षित असतील; निषिद्ध वर्णांवरील आमची माहिती पहा.</t>
-  </si>
-  <si>
-    <t>ऑडसिटी प्रोजेक्ट जतन करताना फाईल&gt; सेव्ह प्रोजेक्ट कमांडचा वापर करणे सहसा सर्वात सोपा आहे, ज्यामध्ये सीटीआरएल + एस (किंवा मॅकवर ⌘ + एस) चा डीफॉल्ट शॉर्टकट आहे. आपण यामध्ये आणखी बदल करुन एखादा प्रकल्प पुन्हा जतन केल्यास, "प्रकल्प जतन करा" नंतर प्रॉमप्ट्सचा त्रास न घेता .aup फाइल आणि _डेटा फोल्डर शांतपणे अद्यतनित करते.</t>
-  </si>
-  <si>
-    <t>प्रोजेक्टमध्ये कोणतेही जतन न केलेले बदल नसल्यास (उदाहरणार्थ, प्रकल्प रिक्त असल्यास किंवा आपण नुकताच जतन केला असेल तर), "प्रकल्प जतन करा" राखाडी होईल. त्या प्रकरणात, त्याऐवजी फाइल&gt; प्रकल्प जतन करा&gt; प्रकल्पाची लॉसलेस कॉपी जतन करा ... किंवा फाइल&gt; प्रकल्प म्हणून जतन करा ... वापरा.</t>
-  </si>
-  <si>
-    <t>"प्रोजेक्टची लॉसलेस कॉपी कॉपी करा" हा प्रकल्प नावाची किंवा वेगळ्या ठिकाणी प्रकल्पाची एक प्रत बॅकअप प्रत म्हणून किंवा अनेक वाढीव प्रतींपैकी एक म्हणून बनविण्याचा सुरक्षित आणि शिफारस केलेला मार्ग आहे. राज्यातील प्रकल्प ज्याची विशिष्ट तारीख व वेळ होती.</t>
-  </si>
-  <si>
-    <t>ऑडसिटी द्वारे तयार केल्याप्रमाणे .aup फाइल आणि _डेटा फोल्डर नेहमीच एकत्र ठेवणे आवश्यक आहे. त्यांची सामग्री व्यक्तिचलितपणे कधीही हलवू नका, नाव बदला किंवा बदलू नका. आपली अंतिम निर्यात केलेली फाईल आपल्याला पाहिजे तितक्या होईपर्यंत त्यांना हटवू नका.</t>
-  </si>
-  <si>
     <t>आपण नंतर आपल्या प्रकल्पात परत येत असल्यास, आपण सोडण्यापूर्वी लॉसलेस बॅकअप WAV किंवा AIFF फाईल (किंवा फाइल्स) निर्यात करणे नेहमीच एक समझदार खबरदारी आहे.</t>
   </si>
   <si>
-    <t>जतन केलेला प्रकल्प केवळ ऑडसिटीद्वारे उघडला आणि वापरला जाऊ शकतो; आपल्याला आपल्या ऑडिओ फाइलची इच्छा असल्यास जी आपल्या संगीत प्लेयरवर प्ले होईल किंवा सीडी बर्न करायची असल्यास आपल्याला ती निर्यात करणे आवश्यक आहे.</t>
-  </si>
-  <si>
     <t>उघडा</t>
   </si>
   <si>
     <t>जतन केलेला प्रकल्प पुन्हा उघडण्यासाठी:</t>
   </si>
   <si>
-    <t>फाईल निवडा&gt; उघडा ...</t>
-  </si>
-  <si>
-    <t>किंवा फाइल&gt; अलीकडील फायली वापरा आणि .aup फाइल उघडा.</t>
-  </si>
-  <si>
-    <t>ऑडसिटी प्रोजेक्ट्सबद्दल अधिक वाचा.</t>
-  </si>
-  <si>
-    <t>| &lt;परत: प्रारंभ करणे</t>
+    <t>जतन करणे - ओड्यासिटी माहितीपुस्तिका</t>
+  </si>
+  <si>
+    <t>जतन करणे</t>
+  </si>
+  <si>
+    <t>ओड्यासिटी विकास माहितीपुस्तिकेकडून</t>
+  </si>
+  <si>
+    <t>येथे जा: निर्देशक, शोधा</t>
+  </si>
+  <si>
+    <t>ओड्यासिटीमधील आपल्या अपूर्ण कामात पुन्हा परत येण्यासाठी सर्व गीतपट्टे  आणि संपादने आपण सोडल्यामुळे ओड्यासिटी प्रकल्प  &lt;b&gt; जतन करा &lt;/ b&gt;</t>
+  </si>
+  <si>
+    <t>आपले सध्याचे कार्य अन्य मीडिया अनुप्रयोगांमध्ये सुरु करण्यासाठी किंवा आपले कार्य इतरांकडे पाठवण्यासाठी  आहे &lt;/a&gt;, आपल्याला &lt;b&gt; &lt;a href="export.html "शीर्षक="Export"&gt; निर्यात &lt;/a&gt; आवश्यक आहे</t>
+  </si>
+  <si>
+    <t>आपणास धारिका जतन करण्यात समस्या येत असल्यास  प्रकल्प जतन करण्याबद्दल नेहमी विचारले जाणारे प्रश्न  जे काही वारंवार विचारण्यात येणार्‍या प्रश्नांची उत्तरे देते.</t>
+  </si>
+  <si>
+    <t>धारिका  &gt; जतन प्रकल्प&gt;ा&gt; प्रकल्पाची  लॉसलेस नक्कल  जतन करा ... &lt;/a&gt; &lt;/span&gt; आपल्‍या विद्यमान प्रकल्पाला  &lt;b&gt; नवीन &lt;/ b&gt; नावाने जतन करू देते, आपला विद्यमान प्रकल्प सतत संपादनासाठी खुला ठेवून.</t>
+  </si>
+  <si>
+    <t>धारिका  &gt; जतन प्रकल्प&gt;प्रकल्प जतन करताना प्रकल्प धारिका आणि निर्देशिका ज्यामध्ये धारिका आहे</t>
+  </si>
+  <si>
+    <t>धारिका  &gt; जतन प्रकल्&gt; प्रकल्प म्हणून जतन करा आपल्याला विद्यमान प्रकल्प  नवीन  नावाने जतन करू देते, नवीन प्रकल्प उघडेल आणि जुना प्रकल्प बंद करेल.</t>
+  </si>
+  <si>
+    <t>हे .aup धारिका आणि _डेटा निर्देशिका  जतन करते किंवा अद्यतनित करते. प्रकल्प  जतन   करणे आपल्याला सर्व संपादने आणि ध्वनीमुद्रण  केलेले /आयातित गीतपट्टासह , अपूर्ण काम वाचवू देते आणि नंतर ओड्यासिटीमध्ये जसे होते तसे होते तसेच (पूर्ववत इतिहास वगळता) पुन्हा उघडू देते. कोणत्याही प्रकारची धारिका  जतन प्रमाणे, काही अक्षरे .aup धारिकेच्या च्या नावावर वापरता येणार नाहीत जर त्या ऑपरेटिंग सिस्टमसाठी आरक्षित असतील; &lt;a href="faq_opening_and_saving_files.html#illegal" title="FAQ:Opening and Saving Files"&gt; निषिद्ध वर्ण &lt;/a&gt; वर आमची माहिती पहा.ऑडसेटमध्ये जसे होते तसे होते तसेच (पूर्ववत इतिहास वगळता) पुन्हा उघडू देते. कोणत्याही प्रकारची फाईल सेव्हिंग प्रमाणे, काही अक्षरे .aup फाईलच्या नावावर वापरता येणार नाहीत जर त्या ऑपरेटिंग सिस्टमसाठी आरक्षित असतील; निषिद्ध वर्णांवरील आमची माहिती पहा.</t>
+  </si>
+  <si>
+    <t>ओड्यासिटी प्रकल्प जतन  करताना सामान्यत: धारिका वापरणे सोपे असते धारिका&gt; आज्ञा , ज्याचा पूर्वनिर्धारित आडमार्ग आहे आपण यामध्ये आणखी बदल करुन एखादा प्रकल्प पुन्हा जतन केल्यास, "प्रकल्प जतन करा" नंतर  त्रास न घेता .aup धारिका  आणि _डेटा निर्देशिका शांतपणे अद्यतनित करते.</t>
+  </si>
+  <si>
+    <t>जतन केलेला प्रकल्प केवळ ओड्यासिटीद्वारे उघडला आणि वापरला जाऊ शकतो; आपल्याला आपल्या ध्वनी  धारिका    आपल्या संगीत प्लेयरवर सुरु  करण्याची इच्छा असल्यास किंवा  एखादी सीडी तयार  करायची असेल तर आपल्याला &lt;a href="export.html "शीर्षक="Export"&gt; निर्यात &lt;/a&gt; करावे लागेल. &lt;/li&gt; &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">प्रकल्पामध्ये  कोणतेही जतन न केलेले बदल नसल्यास (उदाहरणार्थ, प्रकल्प रिक्त असल्यास किंवा आपण नुकताच जतन केला असेल तर), "प्रकल्प जतन करा" राखाडी होईल. अशावेळी वापरा   </t>
+  </si>
+  <si>
+    <t>प्रकल्पाची  लॉसलेस नक्कल  जतन करा ...त्याऐवजी प्रकल्प जतन करा ... &lt;/a&gt; &lt;/span&gt;.</t>
+  </si>
+  <si>
+    <t>ओड्यासिटी &lt; b&gt; ने तयार केल्याप्रमाणे .aup धारिका  आणि _डेटा निर्देशिका  नेहमीच एकत्र ठेवणे आवश्यक आहे. त्यांची सामग्री व्यक्तिचलितपणे कधीही हलवू नका, नाव बदला किंवा सामग्री  बदलू नका. आपली अंतिम निर्यात केलेली धारिका आपल्या इच्छेनुसार होईपर्यंत त्यांना हटवू नका. &lt;/ Li&gt;</t>
+  </si>
+  <si>
+    <t>धारिका निवडा&gt; उघडा ...</t>
+  </si>
+  <si>
+    <t>किंवा धारिका &gt; अलीकडील धारिका वापरा आणि .aup धारिका उघडा.</t>
+  </si>
+  <si>
+    <t>ओड्यासिटी बद्दल अधिक वाचा</t>
+  </si>
+  <si>
+    <t>परत: प्रारंभ करणे</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +196,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,17 +245,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -285,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,9 +346,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,6 +381,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -526,14 +557,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,40 +577,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -582,10 +618,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -593,10 +629,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -604,10 +640,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -615,10 +651,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -626,10 +662,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -637,10 +673,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -648,10 +684,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -659,10 +695,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -670,10 +706,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -681,10 +717,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -692,10 +728,10 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -703,10 +739,10 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -714,10 +750,10 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -725,10 +761,10 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -736,10 +772,10 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -747,10 +783,10 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -758,10 +794,10 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -769,10 +805,10 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -783,7 +819,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -794,7 +830,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -805,7 +841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -818,5 +854,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>